<commit_message>
General updates and debug
</commit_message>
<xml_diff>
--- a/data/standards/13CThr_standards/13CThr_standards_13C.xlsx
+++ b/data/standards/13CThr_standards/13CThr_standards_13C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aj286/repos/nmr-cdiff/data/standards/13CThr_standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F11858-6EBB-EF41-8957-8D5859F7E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1339C6-9AE7-7041-9DFB-09ADA7BEBB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="3680" windowWidth="26840" windowHeight="15940" xr2:uid="{B7D9A5E1-FE37-3249-BDA6-4DA64D8B4532}"/>
+    <workbookView xWindow="38200" yWindow="2640" windowWidth="26840" windowHeight="15940" xr2:uid="{B7D9A5E1-FE37-3249-BDA6-4DA64D8B4532}"/>
   </bookViews>
   <sheets>
     <sheet name="area" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Time</t>
   </si>
@@ -57,6 +57,39 @@
   </si>
   <si>
     <t>2-aminobutyrate</t>
+  </si>
+  <si>
+    <t>S6B</t>
+  </si>
+  <si>
+    <t>S6C</t>
+  </si>
+  <si>
+    <t>S7A</t>
+  </si>
+  <si>
+    <t>S7B</t>
+  </si>
+  <si>
+    <t>S7C</t>
+  </si>
+  <si>
+    <t>S8A</t>
+  </si>
+  <si>
+    <t>S8B</t>
+  </si>
+  <si>
+    <t>S8C</t>
+  </si>
+  <si>
+    <t>S9A</t>
+  </si>
+  <si>
+    <t>S9B</t>
+  </si>
+  <si>
+    <t>S9C</t>
   </si>
 </sst>
 </file>
@@ -115,10 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E626021C-3AD2-B74E-9B68-A0455AE3C5DF}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -466,336 +502,247 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>204.00439336510831</v>
+        <v>387.10274285488327</v>
       </c>
       <c r="C2">
-        <v>267.13385683064422</v>
+        <v>205.7176567972964</v>
       </c>
       <c r="D2">
-        <v>63.374815465419189</v>
+        <v>198.62592514761761</v>
       </c>
       <c r="E2">
-        <v>42.002617845819977</v>
+        <v>223.3717826938211</v>
       </c>
       <c r="F2">
-        <v>42.002617845819977</v>
+        <v>223.3717826938211</v>
+      </c>
+      <c r="G2">
+        <v>335.61938292098972</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0.94888888888888889</v>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>100.113129690477</v>
+        <v>421.68208689166107</v>
       </c>
       <c r="C3">
-        <v>122.0462328060932</v>
+        <v>217.22113697330741</v>
       </c>
       <c r="D3">
-        <v>40.907324048111697</v>
+        <v>209.77839767663031</v>
       </c>
       <c r="E3">
-        <v>26.425477191761129</v>
+        <v>251.67148318818681</v>
       </c>
       <c r="F3">
-        <v>26.425477191761129</v>
+        <v>251.67148318818681</v>
+      </c>
+      <c r="G3">
+        <v>363.24521868959278</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>120.7694444444444</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>194.14971007058</v>
+        <v>540.77553395833513</v>
       </c>
       <c r="C4">
-        <v>199.9285814112726</v>
+        <v>287.31180987735928</v>
       </c>
       <c r="D4">
-        <v>66.203764788063665</v>
+        <v>251.29832351666889</v>
       </c>
       <c r="E4">
-        <v>48.656344914674769</v>
+        <v>302.10436743737142</v>
       </c>
       <c r="F4">
-        <v>48.656344914674769</v>
+        <v>302.10436743737142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>141.74583333333331</v>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>158.80225872549229</v>
+        <v>439.15175601781749</v>
       </c>
       <c r="C5">
-        <v>139.06590523530289</v>
+        <v>228.20451948081239</v>
       </c>
       <c r="D5">
-        <v>92.458886800616767</v>
+        <v>218.82380169525871</v>
       </c>
       <c r="E5">
-        <v>80.162677683688486</v>
+        <v>256.14203635827988</v>
       </c>
       <c r="F5">
-        <v>80.162677683688486</v>
+        <v>256.14203635827988</v>
+      </c>
+      <c r="G5">
+        <v>368.00479003856401</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>143.49472222222221</v>
+      <c r="A6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>156.87767550365129</v>
+        <v>520.5700992550851</v>
       </c>
       <c r="C6">
-        <v>211.92048479132089</v>
+        <v>275.3277264097095</v>
       </c>
       <c r="D6">
-        <v>90.818930327193712</v>
-      </c>
-      <c r="E6">
-        <v>111.88709658795381</v>
-      </c>
-      <c r="F6">
-        <v>111.88709658795381</v>
+        <v>266.84663240758948</v>
       </c>
       <c r="G6">
-        <v>77.819362589049319</v>
+        <v>421.39695682750062</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>144.85944444444439</v>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>161.61955309081321</v>
+        <v>248.5690986835809</v>
       </c>
       <c r="C7">
-        <v>237.36375707776151</v>
+        <v>126.9832933903416</v>
       </c>
       <c r="D7">
-        <v>90.92846323856088</v>
+        <v>118.56099442310899</v>
       </c>
       <c r="E7">
-        <v>105.8825063283569</v>
+        <v>145.8130002633703</v>
       </c>
       <c r="F7">
-        <v>105.8825063283569</v>
+        <v>145.8130002633703</v>
       </c>
       <c r="G7">
-        <v>88.543579473056852</v>
+        <v>221.5462773390461</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>154.94055555555559</v>
+      <c r="A8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>96.523867017089884</v>
+        <v>238.27814762368061</v>
       </c>
       <c r="C8">
-        <v>230.36229264655799</v>
+        <v>121.1891007702508</v>
       </c>
       <c r="D8">
-        <v>122.7082046716458</v>
+        <v>125.84982429958789</v>
       </c>
       <c r="E8">
-        <v>155.99464196007111</v>
+        <v>145.0420896361681</v>
       </c>
       <c r="F8">
-        <v>155.99464196007111</v>
+        <v>145.0420896361681</v>
       </c>
       <c r="G8">
-        <v>32.381891967756772</v>
+        <v>203.3826807023045</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>168.17055555555561</v>
+      <c r="A9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>112.484502367261</v>
+        <v>220.59259291247699</v>
       </c>
       <c r="C9">
-        <v>195.33087888188811</v>
+        <v>126.153638294213</v>
       </c>
       <c r="D9">
-        <v>132.9826933863707</v>
+        <v>118.5574150013292</v>
       </c>
       <c r="E9">
-        <v>156.16047030510899</v>
+        <v>138.33161325491849</v>
       </c>
       <c r="F9">
-        <v>156.16047030510899</v>
+        <v>138.33161325491849</v>
       </c>
       <c r="G9">
-        <v>78.319250610485597</v>
+        <v>187.04178091579891</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>169.42555555555549</v>
+      <c r="A10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>107.5395142949653</v>
+        <v>387.76009399357253</v>
       </c>
       <c r="C10">
-        <v>199.7847418547008</v>
+        <v>134.03301863492169</v>
       </c>
       <c r="D10">
-        <v>133.46525390082959</v>
+        <v>126.0619083520201</v>
       </c>
       <c r="E10">
-        <v>158.08163681136509</v>
+        <v>141.2538767799247</v>
       </c>
       <c r="F10">
-        <v>158.08163681136509</v>
+        <v>141.2538767799247</v>
       </c>
       <c r="G10">
-        <v>63.539423520570907</v>
+        <v>227.5563548774123</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>321.80250000000001</v>
+      <c r="A11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>519.4148045644165</v>
+        <v>314.99259272392288</v>
       </c>
       <c r="C11">
-        <v>155.89126318951469</v>
+        <v>102.6128723654552</v>
       </c>
       <c r="D11">
-        <v>231.63200938921631</v>
+        <v>95.043938512659821</v>
       </c>
       <c r="E11">
-        <v>348.24759478212201</v>
+        <v>95.950819923426593</v>
       </c>
       <c r="F11">
-        <v>348.24759478212201</v>
+        <v>95.950819923426593</v>
       </c>
       <c r="G11">
-        <v>380.37688749698782</v>
+        <v>176.21300915547161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>333.79</v>
+      <c r="A12" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>387.10274285488327</v>
+        <v>321.08718991375179</v>
       </c>
       <c r="C12">
-        <v>205.7176567972964</v>
+        <v>113.9192258188824</v>
       </c>
       <c r="D12">
-        <v>198.62592514761761</v>
+        <v>109.4813513621831</v>
       </c>
       <c r="E12">
-        <v>223.3717826938211</v>
+        <v>121.1393884271377</v>
       </c>
       <c r="F12">
-        <v>223.3717826938211</v>
+        <v>121.1393884271377</v>
       </c>
       <c r="G12">
-        <v>335.61938292098972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>335.18222222222221</v>
-      </c>
-      <c r="B13">
-        <v>421.68208689166107</v>
-      </c>
-      <c r="C13">
-        <v>217.22113697330741</v>
-      </c>
-      <c r="D13">
-        <v>209.77839767663031</v>
-      </c>
-      <c r="E13">
-        <v>251.67148318818681</v>
-      </c>
-      <c r="F13">
-        <v>251.67148318818681</v>
-      </c>
-      <c r="G13">
-        <v>363.24521868959278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>336.58472222222218</v>
-      </c>
-      <c r="B14">
-        <v>540.77553395833513</v>
-      </c>
-      <c r="C14">
-        <v>287.31180987735928</v>
-      </c>
-      <c r="D14">
-        <v>251.29832351666889</v>
-      </c>
-      <c r="E14">
-        <v>302.10436743737142</v>
-      </c>
-      <c r="F14">
-        <v>302.10436743737142</v>
-      </c>
-      <c r="G14">
-        <v>465.39699218053909</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>338.42305555555549</v>
-      </c>
-      <c r="B15">
-        <v>439.15175601781749</v>
-      </c>
-      <c r="C15">
-        <v>228.20451948081239</v>
-      </c>
-      <c r="D15">
-        <v>218.82380169525871</v>
-      </c>
-      <c r="E15">
-        <v>256.14203635827988</v>
-      </c>
-      <c r="F15">
-        <v>256.14203635827988</v>
-      </c>
-      <c r="G15">
-        <v>368.00479003856401</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>339.92944444444453</v>
-      </c>
-      <c r="B16">
-        <v>520.5700992550851</v>
-      </c>
-      <c r="C16">
-        <v>275.3277264097095</v>
-      </c>
-      <c r="D16">
-        <v>266.84663240758948</v>
-      </c>
-      <c r="E16">
-        <v>301.85541223252329</v>
-      </c>
-      <c r="F16">
-        <v>301.85541223252329</v>
-      </c>
-      <c r="G16">
-        <v>421.39695682750062</v>
+        <v>175.20846845761881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>